<commit_message>
Implementação dos parametros do parceiro Gold validado
</commit_message>
<xml_diff>
--- a/Implementação de lógica de Comissionamento.xlsx
+++ b/Implementação de lógica de Comissionamento.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheus\Documents\MeusProgramasPy\data_partners_request\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{38C6D16D-45F6-41F3-BF82-C66B266356CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9FD080C4-D327-4113-AAE8-E95B528B2A99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9209E4F5-595D-420C-9FBC-FA0F8C09C9BA}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9209E4F5-595D-420C-9FBC-FA0F8C09C9BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="23">
   <si>
     <t>Nome da Parceria</t>
   </si>
@@ -146,14 +146,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -491,7 +490,8 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,7 +610,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -743,177 +743,201 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="3">
         <v>4</v>
       </c>
-      <c r="C8" s="1">
-        <v>0.15</v>
-      </c>
-      <c r="D8" s="1">
+      <c r="C8" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="D8" s="4">
         <v>0.3</v>
       </c>
-      <c r="E8" s="2">
-        <v>0</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="E8" s="5">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="2">
-        <v>0</v>
-      </c>
-      <c r="H8" s="2">
-        <v>0</v>
-      </c>
-      <c r="I8" t="s">
-        <v>12</v>
+      <c r="G8" s="5">
+        <v>0</v>
+      </c>
+      <c r="H8" s="5">
+        <v>0</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="3">
         <v>4</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="4">
         <v>0.2</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="4">
         <v>1</v>
       </c>
-      <c r="E9" s="2">
-        <v>0</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="E9" s="5">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="2">
-        <v>0</v>
-      </c>
-      <c r="H9" s="2">
-        <v>0</v>
-      </c>
-      <c r="I9" t="s">
-        <v>12</v>
+      <c r="G9" s="5">
+        <v>0</v>
+      </c>
+      <c r="H9" s="5">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="3">
         <v>4</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="4">
         <v>0.25</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="4">
         <v>2</v>
       </c>
-      <c r="E10" s="2">
-        <v>0</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="E10" s="5">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G10" s="2">
-        <v>0</v>
-      </c>
-      <c r="H10" s="2">
-        <v>0</v>
-      </c>
-      <c r="I10" t="s">
+      <c r="G10" s="5">
+        <v>0</v>
+      </c>
+      <c r="H10" s="5">
+        <v>0</v>
+      </c>
+      <c r="I10" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="3">
         <v>4</v>
       </c>
-      <c r="C11" s="1">
-        <v>0.15</v>
-      </c>
-      <c r="D11" s="1">
-        <v>0.15</v>
-      </c>
-      <c r="E11" s="2">
-        <v>0</v>
-      </c>
-      <c r="F11" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H11" s="2">
-        <v>0</v>
-      </c>
-      <c r="I11" t="s">
-        <v>12</v>
+      <c r="C11" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="E11" s="5">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="5">
+        <v>0.15</v>
+      </c>
+      <c r="H11" s="5">
+        <v>0</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="3">
         <v>4</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="4">
         <v>0.2</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="4">
         <v>0.85</v>
       </c>
-      <c r="E12" s="2">
-        <v>0</v>
-      </c>
-      <c r="F12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H12" s="2">
-        <v>0</v>
-      </c>
-      <c r="I12" t="s">
-        <v>12</v>
+      <c r="E12" s="5">
+        <v>0</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="5">
+        <v>0.15</v>
+      </c>
+      <c r="H12" s="5">
+        <v>0</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="3">
         <v>4</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="4">
         <v>0.25</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="4">
         <v>1.7</v>
       </c>
-      <c r="E13" s="2">
-        <v>0</v>
-      </c>
-      <c r="F13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" s="2">
+      <c r="E13" s="5">
+        <v>0</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="5">
         <v>0.3</v>
       </c>
-      <c r="H13" s="2">
-        <v>0</v>
-      </c>
-      <c r="I13" t="s">
+      <c r="H13" s="5">
+        <v>0</v>
+      </c>
+      <c r="I13" s="3" t="s">
         <v>13</v>
+      </c>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Ajuste a respeito do novo método de comissionamento gold, pediram pra remover ele...
</commit_message>
<xml_diff>
--- a/Implementação de lógica de Comissionamento.xlsx
+++ b/Implementação de lógica de Comissionamento.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheus\Documents\MeusProgramasPy\data_partners_request\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9FD080C4-D327-4113-AAE8-E95B528B2A99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44AF298D-C16A-4569-BE9B-379DB852CF4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9209E4F5-595D-420C-9FBC-FA0F8C09C9BA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9209E4F5-595D-420C-9FBC-FA0F8C09C9BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -491,25 +491,25 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
+      <selection pane="bottomLeft" activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.85546875" customWidth="1"/>
+    <col min="3" max="3" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.88671875" customWidth="1"/>
     <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -544,7 +544,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -577,7 +577,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -610,7 +610,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -643,7 +643,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
@@ -676,7 +676,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
@@ -709,7 +709,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
@@ -742,7 +742,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
@@ -775,7 +775,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
@@ -808,7 +808,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>15</v>
       </c>
@@ -841,7 +841,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>15</v>
       </c>
@@ -874,7 +874,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>15</v>
       </c>
@@ -907,7 +907,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>15</v>
       </c>
@@ -940,7 +940,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -969,7 +969,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -998,7 +998,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1027,7 +1027,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1059,7 +1059,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1091,7 +1091,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1123,7 +1123,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1155,7 +1155,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1187,7 +1187,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -1219,7 +1219,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -1251,12 +1251,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="J24" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>19</v>
       </c>
@@ -1288,12 +1288,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="J26" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>19</v>
       </c>
@@ -1325,7 +1325,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="J28" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
Checkpoint antes de grandes alterações no código
</commit_message>
<xml_diff>
--- a/Implementação de lógica de Comissionamento.xlsx
+++ b/Implementação de lógica de Comissionamento.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheus\Documents\MeusProgramasPy\data_partners_request\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44AF298D-C16A-4569-BE9B-379DB852CF4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{223E7AE9-7A96-4961-9968-7A75FCCF36ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9209E4F5-595D-420C-9FBC-FA0F8C09C9BA}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9209E4F5-595D-420C-9FBC-FA0F8C09C9BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="26">
   <si>
     <t>Nome da Parceria</t>
   </si>
@@ -105,13 +105,22 @@
   </si>
   <si>
     <t>sts Software</t>
+  </si>
+  <si>
+    <t>Deixou de Existir</t>
+  </si>
+  <si>
+    <t>Verificado</t>
+  </si>
+  <si>
+    <t>Stress Test</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,8 +128,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -129,7 +145,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC3C3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -143,22 +170,33 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="9" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bom" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFC3C3"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -487,29 +525,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32C9AFAA-F6AE-43C4-8CBB-02A23AAB0C85}">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I22" sqref="I22"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="32.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.88671875" customWidth="1"/>
-    <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.85546875" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -543,305 +582,335 @@
       <c r="K1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="L1" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="7">
         <v>2</v>
       </c>
-      <c r="C2" s="4">
-        <v>0.15</v>
-      </c>
-      <c r="D2" s="4">
-        <v>0.15</v>
-      </c>
-      <c r="E2" s="5">
-        <v>0</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="C2" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="D2" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="E2" s="9">
+        <v>0</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="5">
-        <v>0.15</v>
-      </c>
-      <c r="H2" s="5">
-        <v>0</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3" t="s">
+      <c r="G2" s="9">
+        <v>0.15</v>
+      </c>
+      <c r="H2" s="9">
+        <v>0</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="L2" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="7">
         <v>2</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="8">
         <v>0.2</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="8">
         <v>0.5</v>
       </c>
-      <c r="E3" s="5">
-        <v>0</v>
-      </c>
-      <c r="F3" s="3" t="s">
+      <c r="E3" s="9">
+        <v>0</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="9">
         <v>0.5</v>
       </c>
-      <c r="H3" s="5">
-        <v>0</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3" t="s">
+      <c r="H3" s="9">
+        <v>0</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="L3" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="7">
         <v>2</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="8">
         <v>0.25</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="8">
         <v>1</v>
       </c>
-      <c r="E4" s="5">
-        <v>0</v>
-      </c>
-      <c r="F4" s="3" t="s">
+      <c r="E4" s="9">
+        <v>0</v>
+      </c>
+      <c r="F4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="9">
         <v>1</v>
       </c>
-      <c r="H4" s="5">
-        <v>0</v>
-      </c>
-      <c r="I4" s="3" t="s">
+      <c r="H4" s="9">
+        <v>0</v>
+      </c>
+      <c r="I4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3" t="s">
+      <c r="J4" s="7"/>
+      <c r="K4" s="7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="L4" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="7">
         <v>3</v>
       </c>
-      <c r="C5" s="4">
-        <v>0.15</v>
-      </c>
-      <c r="D5" s="4">
+      <c r="C5" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="D5" s="8">
         <v>0.25</v>
       </c>
-      <c r="E5" s="5">
-        <v>0</v>
-      </c>
-      <c r="F5" s="3" t="s">
+      <c r="E5" s="9">
+        <v>0</v>
+      </c>
+      <c r="F5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="9">
         <v>0.05</v>
       </c>
-      <c r="H5" s="5">
-        <v>0</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3" t="s">
+      <c r="H5" s="9">
+        <v>0</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="L5" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="7">
         <v>3</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="8">
         <v>0.2</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="8">
         <v>0.85</v>
       </c>
-      <c r="E6" s="5">
-        <v>0</v>
-      </c>
-      <c r="F6" s="3" t="s">
+      <c r="E6" s="9">
+        <v>0</v>
+      </c>
+      <c r="F6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="5">
-        <v>0.15</v>
-      </c>
-      <c r="H6" s="5">
-        <v>0</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3" t="s">
+      <c r="G6" s="9">
+        <v>0.15</v>
+      </c>
+      <c r="H6" s="9">
+        <v>0</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="L6" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="7">
         <v>3</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="8">
         <v>0.25</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="8">
         <v>1.7</v>
       </c>
-      <c r="E7" s="5">
-        <v>0</v>
-      </c>
-      <c r="F7" s="3" t="s">
+      <c r="E7" s="9">
+        <v>0</v>
+      </c>
+      <c r="F7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="9">
         <v>0.3</v>
       </c>
-      <c r="H7" s="5">
-        <v>0</v>
-      </c>
-      <c r="I7" s="3" t="s">
+      <c r="H7" s="9">
+        <v>0</v>
+      </c>
+      <c r="I7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3" t="s">
+      <c r="J7" s="7"/>
+      <c r="K7" s="7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+      <c r="L7" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="7">
         <v>4</v>
       </c>
-      <c r="C8" s="4">
-        <v>0.15</v>
-      </c>
-      <c r="D8" s="4">
+      <c r="C8" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="D8" s="8">
         <v>0.3</v>
       </c>
-      <c r="E8" s="5">
-        <v>0</v>
-      </c>
-      <c r="F8" s="3" t="s">
+      <c r="E8" s="9">
+        <v>0</v>
+      </c>
+      <c r="F8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="5">
-        <v>0</v>
-      </c>
-      <c r="H8" s="5">
-        <v>0</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3" t="s">
+      <c r="G8" s="9">
+        <v>0</v>
+      </c>
+      <c r="H8" s="9">
+        <v>0</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+      <c r="L8" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="7">
         <v>4</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="8">
         <v>0.2</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="8">
         <v>1</v>
       </c>
-      <c r="E9" s="5">
-        <v>0</v>
-      </c>
-      <c r="F9" s="3" t="s">
+      <c r="E9" s="9">
+        <v>0</v>
+      </c>
+      <c r="F9" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="5">
-        <v>0</v>
-      </c>
-      <c r="H9" s="5">
-        <v>0</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3" t="s">
+      <c r="G9" s="9">
+        <v>0</v>
+      </c>
+      <c r="H9" s="9">
+        <v>0</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+      <c r="L9" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="7">
         <v>4</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="8">
         <v>0.25</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="8">
         <v>2</v>
       </c>
-      <c r="E10" s="5">
-        <v>0</v>
-      </c>
-      <c r="F10" s="3" t="s">
+      <c r="E10" s="9">
+        <v>0</v>
+      </c>
+      <c r="F10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G10" s="5">
-        <v>0</v>
-      </c>
-      <c r="H10" s="5">
-        <v>0</v>
-      </c>
-      <c r="I10" s="3" t="s">
+      <c r="G10" s="9">
+        <v>0</v>
+      </c>
+      <c r="H10" s="9">
+        <v>0</v>
+      </c>
+      <c r="I10" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3" t="s">
+      <c r="J10" s="7"/>
+      <c r="K10" s="7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L10" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>15</v>
       </c>
@@ -871,10 +940,10 @@
       </c>
       <c r="J11" s="3"/>
       <c r="K11" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>15</v>
       </c>
@@ -904,10 +973,10 @@
       </c>
       <c r="J12" s="3"/>
       <c r="K12" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>15</v>
       </c>
@@ -937,10 +1006,10 @@
       </c>
       <c r="J13" s="3"/>
       <c r="K13" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -969,7 +1038,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -998,7 +1067,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1027,7 +1096,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1059,7 +1128,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1091,7 +1160,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1123,7 +1192,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1155,7 +1224,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1187,7 +1256,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -1219,7 +1288,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -1251,12 +1320,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J24" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>19</v>
       </c>
@@ -1288,12 +1357,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J26" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>19</v>
       </c>
@@ -1325,7 +1394,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J28" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
implementação de parceiros exsat
</commit_message>
<xml_diff>
--- a/Implementação de lógica de Comissionamento.xlsx
+++ b/Implementação de lógica de Comissionamento.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheus\Documents\MeusProgramasPy\data_partners_request\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{223E7AE9-7A96-4961-9968-7A75FCCF36ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23660D9F-5141-4B5A-8164-AA617422C3F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9209E4F5-595D-420C-9FBC-FA0F8C09C9BA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9209E4F5-595D-420C-9FBC-FA0F8C09C9BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="26">
   <si>
     <t>Nome da Parceria</t>
   </si>
@@ -525,11 +525,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32C9AFAA-F6AE-43C4-8CBB-02A23AAB0C85}">
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J16" sqref="J16"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,7 +1096,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1128,7 +1128,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1160,7 +1160,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1192,210 +1192,218 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="7">
         <v>6</v>
       </c>
-      <c r="C20" s="1">
-        <v>0.15</v>
-      </c>
-      <c r="D20" s="1">
-        <v>0.15</v>
-      </c>
-      <c r="E20" s="2">
+      <c r="C20" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="D20" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="E20" s="9">
         <v>0.01</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G20" s="2">
-        <v>0</v>
-      </c>
-      <c r="H20" s="2">
-        <v>0</v>
-      </c>
-      <c r="I20" t="s">
-        <v>12</v>
-      </c>
-      <c r="J20" t="s">
+      <c r="G20" s="9">
+        <v>0</v>
+      </c>
+      <c r="H20" s="9">
+        <v>0</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J20" s="7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="K20" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="7">
         <v>6</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="8">
         <v>0.2</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21" s="8">
         <v>0.5</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="9">
         <v>0.01</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G21" s="2">
-        <v>0</v>
-      </c>
-      <c r="H21" s="2">
-        <v>0</v>
-      </c>
-      <c r="I21" t="s">
-        <v>12</v>
-      </c>
-      <c r="J21" t="s">
+      <c r="G21" s="9">
+        <v>0</v>
+      </c>
+      <c r="H21" s="9">
+        <v>0</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J21" s="7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="K21" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="7">
         <v>6</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22" s="8">
         <v>0.25</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22" s="8">
         <v>1</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="9">
         <v>0.01</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G22" s="2">
-        <v>0</v>
-      </c>
-      <c r="H22" s="2">
-        <v>0</v>
-      </c>
-      <c r="I22" t="s">
+      <c r="G22" s="9">
+        <v>0</v>
+      </c>
+      <c r="H22" s="9">
+        <v>0</v>
+      </c>
+      <c r="I22" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="J22" t="s">
+      <c r="J22" s="7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="K22" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="7">
         <v>6</v>
       </c>
-      <c r="C23" s="1">
-        <v>0.15</v>
-      </c>
-      <c r="D23" s="1">
-        <v>0.15</v>
-      </c>
-      <c r="E23" s="2">
+      <c r="C23" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="D23" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="E23" s="9">
         <v>0.01</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G23" s="9">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="H23" s="2">
-        <v>0</v>
-      </c>
-      <c r="I23" t="s">
-        <v>12</v>
-      </c>
-      <c r="J23" t="s">
+      <c r="H23" s="9">
+        <v>0</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J23" s="7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J24" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="K23" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B25">
+      <c r="B24" s="7">
         <v>6</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C24" s="8">
         <v>0.2</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D24" s="8">
         <v>0.5</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E24" s="9">
         <v>0.01</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F24" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G25" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H25" s="2">
-        <v>0</v>
-      </c>
-      <c r="I25" t="s">
-        <v>12</v>
-      </c>
-      <c r="J25" t="s">
+      <c r="G24" s="9">
+        <v>0.15</v>
+      </c>
+      <c r="H24" s="9">
+        <v>0</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J24" s="7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K24" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="7">
+        <v>6</v>
+      </c>
+      <c r="C25" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="D25" s="8">
+        <v>1</v>
+      </c>
+      <c r="E25" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="H25" s="9">
+        <v>0</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="J25" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="K25" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J26" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>19</v>
-      </c>
-      <c r="B27">
-        <v>6</v>
-      </c>
-      <c r="C27" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="D27" s="1">
-        <v>1</v>
-      </c>
-      <c r="E27" s="2">
-        <v>0.01</v>
-      </c>
-      <c r="F27" t="s">
-        <v>11</v>
-      </c>
-      <c r="G27" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="H27" s="2">
-        <v>0</v>
-      </c>
-      <c r="I27" t="s">
-        <v>13</v>
-      </c>
-      <c r="J27" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J28" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implementação do ajuste de finders que não existem em pipeline 36
</commit_message>
<xml_diff>
--- a/Implementação de lógica de Comissionamento.xlsx
+++ b/Implementação de lógica de Comissionamento.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheus\Documents\MeusProgramasPy\data_partners_request\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8CB7F9F-86EE-44C9-BC8C-A5AE102E3ED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8806C97-795B-4D2F-A626-BEA65D79478B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9209E4F5-595D-420C-9FBC-FA0F8C09C9BA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9209E4F5-595D-420C-9FBC-FA0F8C09C9BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -542,7 +542,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K12" sqref="K12"/>
+      <selection pane="bottomLeft" activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Checkpoint nos ajustes textuais, sendo eles a implementação de: Introdução, Dados Gerais, Métricas de Fechamento e Métricas de Prospecção
</commit_message>
<xml_diff>
--- a/Implementação de lógica de Comissionamento.xlsx
+++ b/Implementação de lógica de Comissionamento.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheus\Documents\MeusProgramasPy\data_partners_request\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8806C97-795B-4D2F-A626-BEA65D79478B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A08C8291-76CB-4EF4-9736-93C50A6C1B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9209E4F5-595D-420C-9FBC-FA0F8C09C9BA}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9209E4F5-595D-420C-9FBC-FA0F8C09C9BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -542,7 +542,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J26" sqref="J26"/>
+      <selection pane="bottomLeft" activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Ajuste na disponibilização das tabelas, agora estão alinhadas de acordo com o espaço das linhas
</commit_message>
<xml_diff>
--- a/Implementação de lógica de Comissionamento.xlsx
+++ b/Implementação de lógica de Comissionamento.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheus\Documents\MeusProgramasPy\data_partners_request\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A08C8291-76CB-4EF4-9736-93C50A6C1B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F80EDE2C-41AC-47B9-B754-992C5096A246}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9209E4F5-595D-420C-9FBC-FA0F8C09C9BA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9209E4F5-595D-420C-9FBC-FA0F8C09C9BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -542,25 +542,25 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K3" sqref="K3"/>
+      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.42578125" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19" customWidth="1"/>
+    <col min="8" max="8" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.44140625" customWidth="1"/>
+    <col min="10" max="10" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -595,7 +595,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -630,7 +630,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -665,7 +665,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -700,7 +700,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -735,7 +735,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -770,7 +770,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -805,7 +805,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -840,7 +840,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -875,7 +875,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -910,7 +910,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>14</v>
       </c>
@@ -945,7 +945,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>14</v>
       </c>
@@ -980,7 +980,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
@@ -1015,7 +1015,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -1050,7 +1050,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
@@ -1085,7 +1085,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -1120,7 +1120,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -1155,7 +1155,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -1190,7 +1190,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
@@ -1225,7 +1225,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
@@ -1260,7 +1260,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>17</v>
       </c>
@@ -1295,7 +1295,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>17</v>
       </c>
@@ -1330,7 +1330,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>17</v>
       </c>
@@ -1365,7 +1365,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>17</v>
       </c>
@@ -1400,7 +1400,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>17</v>
       </c>

</xml_diff>